<commit_message>
Revamp call tickets navigation and tabs
</commit_message>
<xml_diff>
--- a/data/cx_dim_complaint_type.xlsx
+++ b/data/cx_dim_complaint_type.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnemu\Desktop\call_ticket_unify_aug_18\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnemu\Desktop\call_ticket_unify_sep_4\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34678942-147E-4017-9FBE-839ED984FF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE33CE5-C0AD-42BA-A28D-A1DE6F8A76BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19305" yWindow="3180" windowWidth="29100" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7065" yWindow="6690" windowWidth="31260" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Enhance ticket form with new fields and validation
</commit_message>
<xml_diff>
--- a/data/cx_dim_complaint_type.xlsx
+++ b/data/cx_dim_complaint_type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnemu\Desktop\call_ticket_unify_sep_4\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnemu\Desktop\call_ticket_unify_sep_24\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE33CE5-C0AD-42BA-A28D-A1DE6F8A76BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77E7B05-926C-47DF-AEEC-11714FF0B71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="6690" windowWidth="31260" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12555" yWindow="1995" windowWidth="37935" windowHeight="18465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>complaint_type_id</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>Kurdtel</t>
-  </si>
-  <si>
-    <t>Refund</t>
   </si>
 </sst>
 </file>
@@ -98,6 +95,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -442,11 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -592,14 +594,6 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>